<commit_message>
Updated 2007 to 2022 NAICS code crosswalk based on manual fixes done to error contracts for this year's MEIS.
Also shifted files in the raw data folder to deprecated - files are from prior years
</commit_message>
<xml_diff>
--- a/data/raw/2007_to_2022_NAICS.xlsx
+++ b/data/raw/2007_to_2022_NAICS.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumeet.bedi\Documents\R\MEIS_Methodology\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sumeet.bedi\Documents\R\meis_code\meis_pre-implan_activity_sheets\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE99A144-7EFC-4946-98EB-141ABDE0482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28046279-F5B8-4AF1-B873-09B0F119C57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0990EEED-D02E-4EA5-9855-C170BDE5023A}"/>
+    <workbookView xWindow="14760" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0990EEED-D02E-4EA5-9855-C170BDE5023A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,9 +101,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -141,7 +141,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -247,7 +247,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -389,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -397,11 +397,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AF1629-833D-43A6-B765-95F362080690}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -460,40 +463,40 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>332212</v>
+        <v>332116</v>
       </c>
       <c r="B6">
-        <v>332216</v>
+        <v>332119</v>
       </c>
       <c r="C6">
-        <v>332216</v>
+        <v>332119</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>333293</v>
+        <v>332212</v>
       </c>
       <c r="B7">
-        <v>333244</v>
+        <v>332216</v>
       </c>
       <c r="C7">
-        <v>333244</v>
+        <v>332216</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>333313</v>
+        <v>333293</v>
       </c>
       <c r="B8">
-        <v>333318</v>
+        <v>333244</v>
       </c>
       <c r="C8">
-        <v>333310</v>
+        <v>333248</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>333319</v>
+        <v>333313</v>
       </c>
       <c r="B9">
         <v>333318</v>
@@ -504,67 +507,78 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>333518</v>
+        <v>333319</v>
       </c>
       <c r="B10">
-        <v>333519</v>
+        <v>333318</v>
       </c>
       <c r="C10">
-        <v>333519</v>
+        <v>333310</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>334119</v>
+        <v>333518</v>
       </c>
       <c r="B11">
-        <v>334118</v>
+        <v>333519</v>
       </c>
       <c r="C11">
-        <v>334118</v>
+        <v>333519</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>334411</v>
+        <v>334119</v>
       </c>
       <c r="B12">
-        <v>334419</v>
+        <v>334118</v>
       </c>
       <c r="C12">
-        <v>334419</v>
+        <v>334118</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>339944</v>
+        <v>334411</v>
       </c>
       <c r="B13">
-        <v>339940</v>
+        <v>334419</v>
       </c>
       <c r="C13">
-        <v>339940</v>
+        <v>334419</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>443120</v>
+        <v>339944</v>
       </c>
       <c r="B14">
-        <v>443142</v>
+        <v>339940</v>
       </c>
       <c r="C14">
-        <v>449210</v>
+        <v>339940</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
+        <v>443120</v>
+      </c>
+      <c r="B15">
+        <v>443142</v>
+      </c>
+      <c r="C15">
+        <v>449210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>514210</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>518210</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>518210</v>
       </c>
     </row>

</xml_diff>